<commit_message>
FIx missing OH result for Peter
</commit_message>
<xml_diff>
--- a/data/2020-03-24/Senior Cubers Worldwide - Weekly Competition - 2020-03-24.xlsx
+++ b/data/2020-03-24/Senior Cubers Worldwide - Weekly Competition - 2020-03-24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-03-24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484833C9-0107-4651-B984-62D30AD9AAF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFAE3A6-329F-4CBF-966D-B8192A251A3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3x3x3" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="184">
   <si>
     <t>OH</t>
   </si>
@@ -581,6 +581,9 @@
   <si>
     <t>2:25.26</t>
   </si>
+  <si>
+    <t>1:52.40</t>
+  </si>
 </sst>
 </file>
 
@@ -944,14 +947,14 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="47" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="10" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="47" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -14900,8 +14903,8 @@
   </sheetPr>
   <dimension ref="A1:M1045"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13:I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -15229,8 +15232,8 @@
       <c r="G10" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="H10" s="77">
-        <v>1.3003472222222223E-3</v>
+      <c r="H10" s="80" t="s">
+        <v>183</v>
       </c>
       <c r="I10" s="19" t="s">
         <v>81</v>
@@ -25748,7 +25751,7 @@
   </sheetPr>
   <dimension ref="A1:M1057"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -25996,7 +25999,7 @@
       <c r="C8" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="78" t="s">
+      <c r="D8" s="77" t="s">
         <v>182</v>
       </c>
       <c r="E8" s="26" t="s">
@@ -34903,12 +34906,12 @@
       <c r="A1" s="68" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
       <c r="F1" s="69"/>
     </row>
     <row r="2" spans="1:7" ht="12.75">

</xml_diff>